<commit_message>
4-updated and modified script
</commit_message>
<xml_diff>
--- a/Resources/4-Automatic_PO_Rec.xlsx
+++ b/Resources/4-Automatic_PO_Rec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>WH_NUMBER</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>1658527</t>
+  </si>
+  <si>
+    <t>XX-SUPOP</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -448,11 +451,11 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1658519</v>
+      <c r="B2" s="2">
+        <v>2017112</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>

</xml_diff>

<commit_message>
4-Updated readtext and resource
</commit_message>
<xml_diff>
--- a/Resources/4-Automatic_PO_Rec.xlsx
+++ b/Resources/4-Automatic_PO_Rec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>WH_NUMBER</t>
   </si>
@@ -27,19 +27,7 @@
     <t>06A</t>
   </si>
   <si>
-    <t>1213926</t>
-  </si>
-  <si>
     <t>Item_number</t>
-  </si>
-  <si>
-    <t>1658523</t>
-  </si>
-  <si>
-    <t>1658525</t>
-  </si>
-  <si>
-    <t>1658527</t>
   </si>
 </sst>
 </file>
@@ -417,7 +405,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -434,7 +422,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -449,10 +437,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>1201721</v>
+        <v>1202136</v>
       </c>
       <c r="C2" s="3">
-        <v>1774003</v>
+        <v>1774013</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -466,11 +454,11 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
+      <c r="B3" s="2">
+        <v>1202136</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1774014</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -484,11 +472,11 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
+      <c r="B4" s="2">
+        <v>1202136</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1774015</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -502,11 +490,11 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
+      <c r="B5" s="2">
+        <v>1202136</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1774016</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>

</xml_diff>

<commit_message>
4- added read text
</commit_message>
<xml_diff>
--- a/Resources/4-Automatic_PO_Rec.xlsx
+++ b/Resources/4-Automatic_PO_Rec.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -440,7 +440,7 @@
         <v>1202136</v>
       </c>
       <c r="C2" s="3">
-        <v>1774013</v>
+        <v>1774017</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -458,7 +458,7 @@
         <v>1202136</v>
       </c>
       <c r="C3" s="3">
-        <v>1774014</v>
+        <v>1774018</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -476,7 +476,7 @@
         <v>1202136</v>
       </c>
       <c r="C4" s="3">
-        <v>1774015</v>
+        <v>1774019</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -490,12 +490,8 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
-        <v>1202136</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1774016</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>

</xml_diff>

<commit_message>
4- Updated readtext and resource
</commit_message>
<xml_diff>
--- a/Resources/4-Automatic_PO_Rec.xlsx
+++ b/Resources/4-Automatic_PO_Rec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>WH_NUMBER</t>
   </si>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -438,10 +438,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>1202097</v>
+        <v>1202102</v>
       </c>
       <c r="C2" s="1">
-        <v>1717213</v>
+        <v>1774004</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -459,7 +459,7 @@
         <v>1202102</v>
       </c>
       <c r="C3" s="1">
-        <v>1774004</v>
+        <v>1774005</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -477,7 +477,7 @@
         <v>1202102</v>
       </c>
       <c r="C4" s="1">
-        <v>1774005</v>
+        <v>1774006</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -488,15 +488,9 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1202102</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1774006</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -531,8 +525,8 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -744,18 +738,6 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
4-update data with remaining values
</commit_message>
<xml_diff>
--- a/Resources/4-Automatic_PO_Rec.xlsx
+++ b/Resources/4-Automatic_PO_Rec.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>WH_NUMBER</t>
   </si>
@@ -49,18 +49,12 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -90,13 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -402,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,11 +428,11 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1202102</v>
       </c>
       <c r="C2" s="1">
-        <v>1774004</v>
+        <v>1774009</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -455,11 +446,11 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1202102</v>
       </c>
       <c r="C3" s="1">
-        <v>1774005</v>
+        <v>1774010</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -470,15 +461,9 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1202102</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1774006</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -489,8 +474,8 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -501,8 +486,8 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -513,8 +498,8 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -678,66 +663,6 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>